<commit_message>
Add base statistics to threading analysis
</commit_message>
<xml_diff>
--- a/documentation/Threading Analysis - DDSSA.xlsx
+++ b/documentation/Threading Analysis - DDSSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John_\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A87514-8447-47E5-9A1D-2F57BC1D9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C130C44B-D869-4C3E-8303-98BE7D4EC480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9D00B310-DA03-4259-8009-DDC96E95BBE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="22">
   <si>
     <t>Projects</t>
   </si>
@@ -65,6 +65,45 @@
   </si>
   <si>
     <t>Project Title</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -112,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,11 +159,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -132,18 +180,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2280,15 +2330,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>40957</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>126682</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2656,10 +2706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF1AE8B-15D5-4AAB-8E3A-87B1F85A11BC}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2667,12 +2717,12 @@
     <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2685,21 +2735,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -2722,7 +2772,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2">
@@ -2745,7 +2795,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2">
@@ -2841,11 +2891,304 @@
         <v>61.988221780000003</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="H10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="K10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="9">
+        <v>12.837975139999941</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="9">
+        <v>13.310045840000001</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="9">
+        <v>61.988221780000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9">
+        <v>6.1407099013225774E-2</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.68271194289121306</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0.78205121552279555</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9">
+        <v>12.852055699999999</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9">
+        <v>12.9315113</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="9">
+        <v>61.807760399999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.1373104476946331</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1.5265903133557068</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="9">
+        <v>1.7487196797953097</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1.8854159046100577E-2</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2.3304779848314752</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="9">
+        <v>3.0580205185034108</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="9">
+        <v>-2.9004110861904842</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="9">
+        <v>-2.1987104865845106</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="9">
+        <v>2.9320479765440055E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="9">
+        <v>-0.15017142890443907</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.48342708153789798</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="9">
+        <v>-0.72700937333999838</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.29082120000010114</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="9">
+        <v>3.4196302999999997</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="9">
+        <v>4.3266662999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="9">
+        <v>12.684070499999899</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="9">
+        <v>11.890037299999999</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="9">
+        <v>59.381199899999999</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="9">
+        <v>12.974891700000001</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="9">
+        <v>15.309667599999999</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="9">
+        <v>63.707866199999998</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="9">
+        <v>64.189875699999703</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="9">
+        <v>66.550229200000004</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="9">
+        <v>309.94110890000002</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="10">
+        <v>5</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="10">
+        <v>5</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2854,10 +3197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B887EC98-BF57-4A7D-8138-A570C58097D4}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,11 +3208,11 @@
     <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.140625" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2883,21 +3226,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -2920,7 +3263,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2">
@@ -2943,7 +3286,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2">
@@ -3039,11 +3382,296 @@
         <v>59.920816919999957</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="H10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="K10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="9">
+        <v>12.81473076</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="9">
+        <v>12.27770189999994</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="9">
+        <v>59.920816919999957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9">
+        <v>6.8238697277942045E-2</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.18619888464564643</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1.4269666396657912</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9">
+        <v>12.866881599999999</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9">
+        <v>12.183772399999899</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="9">
+        <v>59.699238699999903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.1525863658095083</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.41635336340230727</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="9">
+        <v>3.1907944079171568</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="9">
+        <v>2.3282599030953081E-2</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0.17335012321641374</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="9">
+        <v>10.1811689535954</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="9">
+        <v>-0.91414599591021695</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="9">
+        <v>3.9779368936156096</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="9">
+        <v>-0.92922296359575984</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="9">
+        <v>-0.18390177263246901</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="9">
+        <v>1.9424470222992449</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="9">
+        <v>-0.41435237650715206</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.39161330000000127</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1.0228388000000006</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="9">
+        <v>7.8799684999999968</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="9">
+        <v>12.615308799999999</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="9">
+        <v>11.9795499999999</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="9">
+        <v>55.463803200000001</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="9">
+        <v>13.006922100000001</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="9">
+        <v>13.002388799999901</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="9">
+        <v>63.343771699999998</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="9">
+        <v>64.073653800000002</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="9">
+        <v>61.388509499999699</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="9">
+        <v>299.60408459999979</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="10">
+        <v>5</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="10">
+        <v>5</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="10">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3081,21 +3709,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -3118,7 +3746,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2">
@@ -3135,7 +3763,7 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2">
@@ -3248,21 +3876,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -3285,7 +3913,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2">
@@ -3302,7 +3930,7 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2">
@@ -3385,6 +4013,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058D141F1C3F5C242B55685702B7EB777" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d75cff0fef329b607ebe4e03804f5ea6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d45fe7e5-9d2d-4ba9-8378-704906c9b2ae" xmlns:ns4="cb59bce2-4b1e-4fb8-a056-56b7ee907b7f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="412dd8f402c6715c7ca69e68a0760b7f" ns3:_="" ns4:_="">
     <xsd:import namespace="d45fe7e5-9d2d-4ba9-8378-704906c9b2ae"/>
@@ -3569,15 +4206,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3585,6 +4213,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EBB6C3-F41B-4029-8711-70E210DF5353}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2856F85-AD05-4897-9F06-CD85EF802698}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3599,14 +4235,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EBB6C3-F41B-4029-8711-70E210DF5353}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>